<commit_message>
feat: added source in exported files
refactor: links
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
+    <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -495,4 +496,23 @@
     <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>source: https://ae-scenario-explorer.cloud.set.kuleuven.be</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
style: info button style: label change for sort default style: eu flag in header style: read more link
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -505,9 +505,21 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>source: https://ae-scenario-explorer.cloud.set.kuleuven.be</v>
+    <row r="1" xml:space="preserve">
+      <c r="A1" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+Source: https://ae-scenario-explorer.cloud.set.kuleuven.be
+Disclaimer:
+This tool is part of a study contracted by the European Commission, DG GROW, on the ‘Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction.’ The views expressed in this document and on the scenario modelling tool web app are the sole responsibility of the authors and do not necessarily reflect the views of the European Commission.
+License and citation:
+This tool has been developed as part of GROW/2022/OP/0005. Courtesy of the European Union, DG GROW. Development authored by Martin Röck, Shadwa Eissa, Benjamin Lesné, and Karen Allacker.
+Licensed under a Creative Commons Attribution-ShareAlike 4.0 (CC BY-SA 4.0) International License. When using or improving this tool or parts of it, consider giving appropriate credit. Cite as:
+Röck M, Eissa S, Lesné B, and Allacker K. “Scenario Modelling Tool - Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction” European Commission DG GROW, 2024. DOI: https://doi.org/10.5281/zenodo.13315281. Web-app available online via: https://ae-scenario-explorer.cloud.set.kuleuven.be
+Contact details:
+We encourage users to get in touch with feedback and/or questions on both the study and the tool:
+    Tool Development Lead, KU Leuven: Martin Röck (martin.roeck@kuleuven.be)
+    European Commission, DG GROW: Philippe Moseley (philippe.moseley@ec.europa.eu)
+An extended list of consortium members and contact details is available via the project website.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: use austria parquet files
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -419,10 +419,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>119.687</v>
+        <v>119.68710703486188</v>
       </c>
       <c r="C2">
-        <v>319.473</v>
+        <v>319.47331104198275</v>
       </c>
     </row>
     <row r="3">
@@ -430,10 +430,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>119.163</v>
+        <v>119.16288691782539</v>
       </c>
       <c r="C3">
-        <v>315.329</v>
+        <v>315.32948722099496</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>119.65</v>
+        <v>119.65008370845369</v>
       </c>
       <c r="C4">
-        <v>307.084</v>
+        <v>307.08429024595165</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>115.46</v>
+        <v>115.46035912077282</v>
       </c>
       <c r="C5">
-        <v>295.116</v>
+        <v>295.11620028256016</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>110.565</v>
+        <v>110.56468275012404</v>
       </c>
       <c r="C6">
-        <v>281.564</v>
+        <v>281.5637429123412</v>
       </c>
     </row>
     <row r="7">
@@ -474,10 +474,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>106.062</v>
+        <v>106.06154966260674</v>
       </c>
       <c r="C7">
-        <v>267.935</v>
+        <v>267.9345929015514</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>101.861</v>
+        <v>101.86143875879341</v>
       </c>
       <c r="C8">
-        <v>253.811</v>
+        <v>253.81099237453978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: new parquet files structure/values
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -408,7 +408,7 @@
         <v>stock_projection_year</v>
       </c>
       <c r="B1" t="str">
-        <v>Non-residential</v>
+        <v>Non-Residential</v>
       </c>
       <c r="C1" t="str">
         <v>Residential</v>
@@ -419,10 +419,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>119.68710703486188</v>
+        <v>5989620461.822261</v>
       </c>
       <c r="C2">
-        <v>319.47331104198275</v>
+        <v>15539725146.071728</v>
       </c>
     </row>
     <row r="3">
@@ -430,10 +430,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>119.16288691782539</v>
+        <v>6189508557.828688</v>
       </c>
       <c r="C3">
-        <v>315.32948722099496</v>
+        <v>15860659116.453512</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>119.65008370845369</v>
+        <v>5731297592.470088</v>
       </c>
       <c r="C4">
-        <v>307.08429024595165</v>
+        <v>15469971370.55126</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>115.46035912077282</v>
+        <v>5604720706.924748</v>
       </c>
       <c r="C5">
-        <v>295.11620028256016</v>
+        <v>15512862022.853907</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>110.56468275012404</v>
+        <v>5374894548.775076</v>
       </c>
       <c r="C6">
-        <v>281.5637429123412</v>
+        <v>15360897580.2493</v>
       </c>
     </row>
     <row r="7">
@@ -474,10 +474,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>106.06154966260674</v>
+        <v>5121955169.398381</v>
       </c>
       <c r="C7">
-        <v>267.9345929015514</v>
+        <v>15157003643.782705</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>101.86143875879341</v>
+        <v>4853096961.886391</v>
       </c>
       <c r="C8">
-        <v>253.81099237453978</v>
+        <v>14928953612.305525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: new parquet files with 27 countries
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -408,7 +408,7 @@
         <v>stock_projection_year</v>
       </c>
       <c r="B1" t="str">
-        <v>Non-Residential</v>
+        <v>Non-residential</v>
       </c>
       <c r="C1" t="str">
         <v>Residential</v>
@@ -419,10 +419,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>5989620461.822261</v>
+        <v>420.5118763716624</v>
       </c>
       <c r="C2">
-        <v>15539725146.071728</v>
+        <v>723.2113187875967</v>
       </c>
     </row>
     <row r="3">
@@ -430,10 +430,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>6189508557.828688</v>
+        <v>417.2098904849987</v>
       </c>
       <c r="C3">
-        <v>15860659116.453512</v>
+        <v>708.340439546219</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>5731297592.470088</v>
+        <v>415.72087345171656</v>
       </c>
       <c r="C4">
-        <v>15469971370.55126</v>
+        <v>699.7582047619915</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>5604720706.924748</v>
+        <v>414.8188235513056</v>
       </c>
       <c r="C5">
-        <v>15512862022.853907</v>
+        <v>691.7742393846</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>5374894548.775076</v>
+        <v>414.5569372331537</v>
       </c>
       <c r="C6">
-        <v>15360897580.2493</v>
+        <v>683.1864284357799</v>
       </c>
     </row>
     <row r="7">
@@ -474,10 +474,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>5121955169.398381</v>
+        <v>415.43283424500953</v>
       </c>
       <c r="C7">
-        <v>15157003643.782705</v>
+        <v>672.3298372900899</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>4853096961.886391</v>
+        <v>417.0907195523708</v>
       </c>
       <c r="C8">
-        <v>14928953612.305525</v>
+        <v>660.3146200847184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: stripe pattern feat: round returned decimals from db
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -419,10 +419,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>420.5118763716624</v>
+        <v>420.511876</v>
       </c>
       <c r="C2">
-        <v>723.2113187875967</v>
+        <v>723.211319</v>
       </c>
     </row>
     <row r="3">
@@ -430,10 +430,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>417.2098904849987</v>
+        <v>417.20989</v>
       </c>
       <c r="C3">
-        <v>708.340439546219</v>
+        <v>708.34044</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>415.72087345171656</v>
+        <v>415.720873</v>
       </c>
       <c r="C4">
-        <v>699.7582047619915</v>
+        <v>699.758205</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>414.8188235513056</v>
+        <v>414.818824</v>
       </c>
       <c r="C5">
-        <v>691.7742393846</v>
+        <v>691.774239</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>414.5569372331537</v>
+        <v>414.556937</v>
       </c>
       <c r="C6">
-        <v>683.1864284357799</v>
+        <v>683.186428</v>
       </c>
     </row>
     <row r="7">
@@ -474,10 +474,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>415.43283424500953</v>
+        <v>415.432834</v>
       </c>
       <c r="C7">
-        <v>672.3298372900899</v>
+        <v>672.329837</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>417.0907195523708</v>
+        <v>417.09072</v>
       </c>
       <c r="C8">
-        <v>660.3146200847184</v>
+        <v>660.31462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: new parquet files doc
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -419,10 +419,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>420.511876</v>
+        <v>267.289004</v>
       </c>
       <c r="C2">
-        <v>723.211319</v>
+        <v>527.785518</v>
       </c>
     </row>
     <row r="3">
@@ -430,10 +430,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>417.20989</v>
+        <v>236.473001</v>
       </c>
       <c r="C3">
-        <v>708.34044</v>
+        <v>488.515772</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>415.720873</v>
+        <v>191.882325</v>
       </c>
       <c r="C4">
-        <v>699.758205</v>
+        <v>414.575915</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>414.818824</v>
+        <v>150.330923</v>
       </c>
       <c r="C5">
-        <v>691.774239</v>
+        <v>323.723967</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>414.556937</v>
+        <v>112.816196</v>
       </c>
       <c r="C6">
-        <v>683.186428</v>
+        <v>231.341876</v>
       </c>
     </row>
     <row r="7">
@@ -474,10 +474,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>415.432834</v>
+        <v>88.552161</v>
       </c>
       <c r="C7">
-        <v>672.329837</v>
+        <v>157.35794</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>417.09072</v>
+        <v>71.030787</v>
       </c>
       <c r="C8">
-        <v>660.31462</v>
+        <v>89.632421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add docker build arg for NODE_ENV feat: consistent hostname for tests
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -508,13 +508,13 @@
     <row r="1" xml:space="preserve">
       <c r="A1" t="str" xml:space="preserve">
         <v xml:space="preserve">
-Source: https://ae-scenario-explorer.cloud.set.kuleuven.be
+Source: https://consistent-url-for-testing.com
 Disclaimer:
 This tool is part of a study contracted by the European Commission, DG GROW, on the ‘Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction.’ The views expressed in this document and on the scenario modelling tool web app are the sole responsibility of the authors and do not necessarily reflect the views of the European Commission.
 License and citation:
 This tool has been developed as part of GROW/2022/OP/0005. Courtesy of the European Union, DG GROW. Development authored by Martin Röck, Shadwa Eissa, Benjamin Lesné, and Karen Allacker.
 Licensed under a Creative Commons Attribution-ShareAlike 4.0 (CC BY-SA 4.0) International License. When using or improving this tool or parts of it, consider giving appropriate credit. Cite as:
-Röck M, Eissa S, Lesné B, and Allacker K. “Scenario Modelling Tool - Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction” European Commission DG GROW, 2024. DOI: https://doi.org/10.5281/zenodo.13315281. Web-app available online via: https://ae-scenario-explorer.cloud.set.kuleuven.be
+Röck M, Eissa S, Lesné B, and Allacker K. “Scenario Modelling Tool - Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction” European Commission DG GROW, 2024. DOI: https://doi.org/10.5281/zenodo.13315281. Web-app available online via: https://consistent-url-for-testing.com
 Contact details:
 We encourage users to get in touch with feedback and/or questions on both the study and the tool:
     Tool Development Lead, KU Leuven: Martin Röck (martin.roeck@kuleuven.be)

</xml_diff>

<commit_message>
feat: scenario parameters / strategy
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -430,10 +430,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>236.473001</v>
+        <v>262.565466</v>
       </c>
       <c r="C3">
-        <v>488.515772</v>
+        <v>507.3796</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>191.882325</v>
+        <v>258.778498</v>
       </c>
       <c r="C4">
-        <v>414.575915</v>
+        <v>493.55589</v>
       </c>
     </row>
     <row r="5">
@@ -452,10 +452,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>150.330923</v>
+        <v>254.88822</v>
       </c>
       <c r="C5">
-        <v>323.723967</v>
+        <v>480.585165</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>112.816196</v>
+        <v>251.481461</v>
       </c>
       <c r="C6">
-        <v>231.341876</v>
+        <v>467.339775</v>
       </c>
     </row>
     <row r="7">
@@ -474,10 +474,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>88.552161</v>
+        <v>248.329292</v>
       </c>
       <c r="C7">
-        <v>157.35794</v>
+        <v>452.586723</v>
       </c>
     </row>
     <row r="8">
@@ -485,10 +485,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>71.030787</v>
+        <v>245.442244</v>
       </c>
       <c r="C8">
-        <v>89.632421</v>
+        <v>437.623499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: migrate from hard coded units to dynamic
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -496,35 +495,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1" xml:space="preserve">
-      <c r="A1" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Source: https://consistent-url-for-testing.com
-Disclaimer:
-This tool is part of a study contracted by the European Commission, DG GROW, on the ‘Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction.’ The views expressed in this document and on the scenario modelling tool web app are the sole responsibility of the authors and do not necessarily reflect the views of the European Commission.
-License and citation:
-This tool has been developed as part of GROW/2022/OP/0005. Courtesy of the European Union, DG GROW. Development authored by Martin Röck, Shadwa Eissa, Benjamin Lesné, and Karen Allacker.
-Licensed under a Creative Commons Attribution-ShareAlike 4.0 (CC BY-SA 4.0) International License. When using or improving this tool or parts of it, consider giving appropriate credit. Cite as:
-Röck M, Eissa S, Lesné B, and Allacker K. “Scenario Modelling Tool - Analysis of Life-cycle Greenhouse Gas Emissions and Removals of EU Buildings and Construction” European Commission DG GROW, 2024. DOI: https://doi.org/10.5281/zenodo.13315281. Web-app available online via: https://consistent-url-for-testing.com
-Contact details:
-We encourage users to get in touch with feedback and/or questions on both the study and the tool:
-    Tool Development Lead, KU Leuven: Martin Röck (martin.roeck@kuleuven.be)
-    European Commission, DG GROW: Philippe Moseley (philippe.moseley@ec.europa.eu)
-An extended list of consortium members and contact details is available via the project website.</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: dynamic ticks on Y axis, dynamic units, new seed data
</commit_message>
<xml_diff>
--- a/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
+++ b/e2e/tests/pages/dashboard/features/download.spec.ts-snapshots/scenario-chromium-linux.xlsx
@@ -418,10 +418,10 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>267.289004</v>
+        <v>3.5856</v>
       </c>
       <c r="C2">
-        <v>527.785518</v>
+        <v>3.5358</v>
       </c>
     </row>
     <row r="3">
@@ -429,10 +429,10 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>262.565466</v>
+        <v>3.5429</v>
       </c>
       <c r="C3">
-        <v>507.3796</v>
+        <v>3.5928</v>
       </c>
     </row>
     <row r="4">
@@ -440,10 +440,10 @@
         <v>2030</v>
       </c>
       <c r="B4">
-        <v>258.778498</v>
+        <v>3.6</v>
       </c>
       <c r="C4">
-        <v>493.55589</v>
+        <v>3.55</v>
       </c>
     </row>
     <row r="5">
@@ -451,10 +451,10 @@
         <v>2035</v>
       </c>
       <c r="B5">
-        <v>254.88822</v>
+        <v>3.5571</v>
       </c>
       <c r="C5">
-        <v>480.585165</v>
+        <v>3.6072</v>
       </c>
     </row>
     <row r="6">
@@ -462,10 +462,10 @@
         <v>2040</v>
       </c>
       <c r="B6">
-        <v>251.481461</v>
+        <v>3.6144</v>
       </c>
       <c r="C6">
-        <v>467.339775</v>
+        <v>3.5642</v>
       </c>
     </row>
     <row r="7">
@@ -473,10 +473,10 @@
         <v>2045</v>
       </c>
       <c r="B7">
-        <v>248.329292</v>
+        <v>3.5713</v>
       </c>
       <c r="C7">
-        <v>452.586723</v>
+        <v>3.6216</v>
       </c>
     </row>
     <row r="8">
@@ -484,10 +484,10 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>245.442244</v>
+        <v>3.5287</v>
       </c>
       <c r="C8">
-        <v>437.623499</v>
+        <v>3.5784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>